<commit_message>
I'm like 80% happy running stats on this.
</commit_message>
<xml_diff>
--- a/data/23 nrec biomass outliers fixed.xlsx
+++ b/data/23 nrec biomass outliers fixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF643A6E-0329-3844-9389-25A0002CFC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A94144-D1D3-114B-B6F9-3DAFF2D9D64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{DAC39784-4BA9-7C42-AA44-06062B55DAF5}"/>
   </bookViews>
@@ -485,8 +485,8 @@
   <dimension ref="A1:K401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J126" sqref="J126"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A219" sqref="A219:XFD219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Put models together into their on dataframes.
</commit_message>
<xml_diff>
--- a/data/23 nrec biomass outliers fixed.xlsx
+++ b/data/23 nrec biomass outliers fixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A94144-D1D3-114B-B6F9-3DAFF2D9D64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F8C3EB-504E-1E40-935C-8CB3CBC23398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{DAC39784-4BA9-7C42-AA44-06062B55DAF5}"/>
   </bookViews>
@@ -485,8 +485,8 @@
   <dimension ref="A1:K401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A219" sqref="A219:XFD219"/>
+      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J368" sqref="J368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13043,7 +13043,7 @@
         <v>0.1</v>
       </c>
       <c r="I365" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J365">
         <v>20.158000000000001</v>
@@ -13113,7 +13113,7 @@
         <v>0.1</v>
       </c>
       <c r="I367" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J367">
         <v>21.318999999999999</v>
@@ -13149,9 +13149,6 @@
       </c>
       <c r="I368" t="s">
         <v>20</v>
-      </c>
-      <c r="J368">
-        <v>22.116</v>
       </c>
       <c r="K368">
         <v>1.907</v>

</xml_diff>